<commit_message>
Corrige les fichiers de test pour passer les customs check
</commit_message>
<xml_diff>
--- a/api/tests/files/canteens/canteens_good.xlsx
+++ b/api/tests/files/canteens/canteens_good.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">siret</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">gestionnaires_additionnels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13002526500013</t>
   </si>
   <si>
     <t xml:space="preserve">A excel canteen</t>
@@ -86,6 +89,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -106,6 +110,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,16 +155,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -289,90 +298,90 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="24.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>37110328971738</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <v>54460</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="3" t="n">
         <v>700</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="3" t="n">
         <v>14000</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout de la nouvelle colonne dans le fichier excel
</commit_message>
<xml_diff>
--- a/api/tests/files/canteens/canteens_good.xlsx
+++ b/api/tests/files/canteens/canteens_good.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">siret</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">gestionnaires_additionnels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre_satellites</t>
   </si>
   <si>
     <t xml:space="preserve">A excel canteen</t>
@@ -86,6 +89,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -106,6 +110,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,16 +155,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -286,93 +299,97 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M17" activeCellId="1" sqref="M1 M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="24.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+    <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
         <v>37110328971738</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="n">
+      <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="n">
         <v>54460</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="4" t="n">
         <v>700</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="4" t="n">
         <v>14000</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="I2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="J2" s="4" t="s">
         <v>16</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve(Imports): Cantines: ajout du champ nombre_satellites (nécessaire pour les CC) (#5803)
Co-authored-by: Charline Laporte <charline.laporte@beta.gouv.fr>
</commit_message>
<xml_diff>
--- a/api/tests/files/canteens/canteens_good.xlsx
+++ b/api/tests/files/canteens/canteens_good.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">siret</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">gestionnaires_additionnels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre_satellites</t>
   </si>
   <si>
     <t xml:space="preserve">A excel canteen</t>
@@ -86,6 +89,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -106,6 +110,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,16 +155,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -286,93 +299,97 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M17" activeCellId="1" sqref="M1 M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="24.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+    <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
         <v>37110328971738</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="n">
+      <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="n">
         <v>54460</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="4" t="n">
         <v>700</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="4" t="n">
         <v>14000</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="I2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="J2" s="4" t="s">
         <v>16</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Met à jour les fichiers de tests avec le nouveau séparateur
</commit_message>
<xml_diff>
--- a/api/tests/files/canteens/canteens_good.xlsx
+++ b/api/tests/files/canteens/canteens_good.xlsx
@@ -1,31 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
-  <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D545AEC2-5098-4793-8E84-C03EDA3E39E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="canteens_good" sheetId="1" r:id="rId1"/>
+    <sheet name="canteens_good" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -36,67 +22,86 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
-    <t>siret</t>
-  </si>
-  <si>
-    <t>nom</t>
-  </si>
-  <si>
-    <t>siret_livreur_repas</t>
-  </si>
-  <si>
-    <t>nombre_repas_jour</t>
-  </si>
-  <si>
-    <t>nombre_repas_an</t>
-  </si>
-  <si>
-    <t>secteurs</t>
-  </si>
-  <si>
-    <t>type_production</t>
-  </si>
-  <si>
-    <t>type_gestion</t>
-  </si>
-  <si>
-    <t>modèle_économique</t>
-  </si>
-  <si>
-    <t>gestionnaires_additionnels</t>
-  </si>
-  <si>
-    <t>nombre_satellites</t>
-  </si>
-  <si>
-    <t>21340172201787</t>
-  </si>
-  <si>
-    <t>A excel canteen</t>
-  </si>
-  <si>
-    <t>Cliniques+Hôpitaux</t>
-  </si>
-  <si>
-    <t>site</t>
-  </si>
-  <si>
-    <t>conceded</t>
-  </si>
-  <si>
-    <t>public</t>
+    <t xml:space="preserve">siret</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">siret_livreur_repas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre_repas_jour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre_repas_an</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secteurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type_production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type_gestion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modèle_économique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gestionnaires_additionnels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre_satellites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21340172201787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A excel canteen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cliniques,Hôpitaux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conceded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">public</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -114,7 +119,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -122,87 +127,115 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18A303"/>
+        <a:srgbClr val="18a303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369A3"/>
+        <a:srgbClr val="0369a3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A33E03"/>
+        <a:srgbClr val="a33e03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8E03A3"/>
+        <a:srgbClr val="8e03a3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="C99C00"/>
+        <a:srgbClr val="c99c00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="C9211E"/>
+        <a:srgbClr val="c9211e"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000EE"/>
+        <a:srgbClr val="0000ee"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551A8B"/>
+        <a:srgbClr val="551a8b"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -255,35 +288,36 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" style="1" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="22.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -318,17 +352,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1">
+    <row r="2" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="4" t="n">
         <v>700</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="4" t="n">
         <v>14000</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -345,9 +379,10 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Corrige les fichiers test d'imports
</commit_message>
<xml_diff>
--- a/api/tests/files/canteens/canteens_good.xlsx
+++ b/api/tests/files/canteens/canteens_good.xlsx
@@ -64,13 +64,13 @@
     <t xml:space="preserve">Cliniques,Hôpitaux</t>
   </si>
   <si>
-    <t xml:space="preserve">site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conceded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">public</t>
+    <t xml:space="preserve">Restaurant avec cuisine sur place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concédée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Public</t>
   </si>
 </sst>
 </file>
@@ -81,7 +81,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -108,6 +108,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,7 +157,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -171,6 +176,14 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -299,7 +312,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -368,13 +381,13 @@
       <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="6" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
improve(Imports): Cantines: amélioration des terminologies du schéma (#5998)
</commit_message>
<xml_diff>
--- a/api/tests/files/canteens/canteens_good.xlsx
+++ b/api/tests/files/canteens/canteens_good.xlsx
@@ -1,31 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
-  <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D545AEC2-5098-4793-8E84-C03EDA3E39E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="canteens_good" sheetId="1" r:id="rId1"/>
+    <sheet name="canteens_good" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -36,67 +22,86 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
-    <t>siret</t>
-  </si>
-  <si>
-    <t>nom</t>
-  </si>
-  <si>
-    <t>siret_livreur_repas</t>
-  </si>
-  <si>
-    <t>nombre_repas_jour</t>
-  </si>
-  <si>
-    <t>nombre_repas_an</t>
-  </si>
-  <si>
-    <t>secteurs</t>
-  </si>
-  <si>
-    <t>type_production</t>
-  </si>
-  <si>
-    <t>type_gestion</t>
-  </si>
-  <si>
-    <t>modèle_économique</t>
-  </si>
-  <si>
-    <t>gestionnaires_additionnels</t>
-  </si>
-  <si>
-    <t>nombre_satellites</t>
-  </si>
-  <si>
-    <t>21340172201787</t>
-  </si>
-  <si>
-    <t>A excel canteen</t>
-  </si>
-  <si>
-    <t>Cliniques+Hôpitaux</t>
-  </si>
-  <si>
-    <t>site</t>
-  </si>
-  <si>
-    <t>conceded</t>
-  </si>
-  <si>
-    <t>public</t>
+    <t xml:space="preserve">siret</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">siret_livreur_repas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre_repas_jour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre_repas_an</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secteurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type_production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type_gestion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modèle_économique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gestionnaires_additionnels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre_satellites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21340172201787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A excel canteen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cliniques,Hôpitaux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conceded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">public</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -114,7 +119,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -122,87 +127,115 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18A303"/>
+        <a:srgbClr val="18a303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369A3"/>
+        <a:srgbClr val="0369a3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A33E03"/>
+        <a:srgbClr val="a33e03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8E03A3"/>
+        <a:srgbClr val="8e03a3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="C99C00"/>
+        <a:srgbClr val="c99c00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="C9211E"/>
+        <a:srgbClr val="c9211e"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000EE"/>
+        <a:srgbClr val="0000ee"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551A8B"/>
+        <a:srgbClr val="551a8b"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -255,35 +288,36 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" style="1" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="22.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -318,17 +352,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1">
+    <row r="2" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="4" t="n">
         <v>700</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="4" t="n">
         <v>14000</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -345,9 +379,10 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
feat(Import): Cantines: remplacer les valeurs anglaises par leur version "verbeuse" française (#6012)
</commit_message>
<xml_diff>
--- a/api/tests/files/canteens/canteens_good.xlsx
+++ b/api/tests/files/canteens/canteens_good.xlsx
@@ -64,13 +64,13 @@
     <t xml:space="preserve">Cliniques,Hôpitaux</t>
   </si>
   <si>
-    <t xml:space="preserve">site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conceded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">public</t>
+    <t xml:space="preserve">Restaurant avec cuisine sur place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concédée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Public</t>
   </si>
 </sst>
 </file>
@@ -81,7 +81,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -108,6 +108,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,7 +157,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -171,6 +176,14 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -299,7 +312,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -368,13 +381,13 @@
       <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="6" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrige les tests d'imports type success
</commit_message>
<xml_diff>
--- a/api/tests/files/canteens/canteens_good.xlsx
+++ b/api/tests/files/canteens/canteens_good.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="canteens_good" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="canteens_good-2" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">siret</t>
   </si>
@@ -50,12 +50,6 @@
   </si>
   <si>
     <t xml:space="preserve">gestionnaires_additionnels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nombre_satellites</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21340172201787</t>
   </si>
   <si>
     <t xml:space="preserve">A excel canteen</t>
@@ -77,16 +71,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -102,17 +94,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -157,33 +138,9 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -309,86 +266,82 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="22.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.75"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>21340172201787</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="D2" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>14000</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="G2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4" t="n">
-        <v>700</v>
-      </c>
-      <c r="E2" s="4" t="n">
-        <v>14000</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="I2" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(Import): Cantines: supprime le type de production "central" et met à jour les champs liés (#6172)
</commit_message>
<xml_diff>
--- a/api/tests/files/canteens/canteens_good.xlsx
+++ b/api/tests/files/canteens/canteens_good.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="canteens_good" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="canteens_good-2" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">siret</t>
   </si>
@@ -50,12 +50,6 @@
   </si>
   <si>
     <t xml:space="preserve">gestionnaires_additionnels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nombre_satellites</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21340172201787</t>
   </si>
   <si>
     <t xml:space="preserve">A excel canteen</t>
@@ -77,16 +71,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -102,17 +94,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -157,33 +138,9 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -309,86 +266,82 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="22.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.75"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>21340172201787</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="D2" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>14000</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="G2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4" t="n">
-        <v>700</v>
-      </c>
-      <c r="E2" s="4" t="n">
-        <v>14000</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="I2" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(Imports): Cantines: renommer "siret_livreur_repas" pour "siret_cuisine_centrale" (#6261)
</commit_message>
<xml_diff>
--- a/api/tests/files/canteens/canteens_good.xlsx
+++ b/api/tests/files/canteens/canteens_good.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">nom</t>
   </si>
   <si>
-    <t xml:space="preserve">siret_livreur_repas</t>
+    <t xml:space="preserve">siret_cuisine_centrale</t>
   </si>
   <si>
     <t xml:space="preserve">nombre_repas_jour</t>
@@ -79,6 +79,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -138,8 +139,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -269,78 +274,78 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="22.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>21340172201787</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>700</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>14000</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Met à jour les tests
</commit_message>
<xml_diff>
--- a/api/tests/files/canteens/canteens_good.xlsx
+++ b/api/tests/files/canteens/canteens_good.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">siret</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">modèle_économique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">groupe_id</t>
   </si>
   <si>
     <t xml:space="preserve">gestionnaires_additionnels</t>
@@ -271,10 +274,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -322,13 +325,16 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>21340172201787</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>700</v>
@@ -337,16 +343,16 @@
         <v>14000</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(Imports): Cantines: ajoute le colonne "groupe_id" (#6273)
</commit_message>
<xml_diff>
--- a/api/tests/files/canteens/canteens_good.xlsx
+++ b/api/tests/files/canteens/canteens_good.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">siret</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">modèle_économique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">groupe_id</t>
   </si>
   <si>
     <t xml:space="preserve">gestionnaires_additionnels</t>
@@ -271,10 +274,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -322,13 +325,16 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>21340172201787</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>700</v>
@@ -337,16 +343,16 @@
         <v>14000</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MAJ test de success avec la nouvelle colonne
</commit_message>
<xml_diff>
--- a/api/tests/files/canteens/canteens_good.xlsx
+++ b/api/tests/files/canteens/canteens_good.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">siret</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">groupe_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">administration_tutelle</t>
   </si>
   <si>
     <t xml:space="preserve">gestionnaires_additionnels</t>
@@ -274,10 +277,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -292,6 +295,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="22.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="27.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -325,8 +329,11 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -334,7 +341,7 @@
         <v>21340172201787</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>700</v>
@@ -343,16 +350,16 @@
         <v>14000</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(Imports): Cantines: déplace la colonne "Administration de tutelle" dans l'import commun (#6318)
</commit_message>
<xml_diff>
--- a/api/tests/files/canteens/canteens_good.xlsx
+++ b/api/tests/files/canteens/canteens_good.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">siret</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">groupe_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">administration_tutelle</t>
   </si>
   <si>
     <t xml:space="preserve">gestionnaires_additionnels</t>
@@ -274,10 +277,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -292,6 +295,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="22.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="27.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -325,8 +329,11 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -334,7 +341,7 @@
         <v>21340172201787</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>700</v>
@@ -343,16 +350,16 @@
         <v>14000</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>